<commit_message>
pre-revision of manual analysis
</commit_message>
<xml_diff>
--- a/results/baseline_cot/arc/manual_task_analysis.xlsx
+++ b/results/baseline_cot/arc/manual_task_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Universität\Mannheim\Studium\5. Semester HWS\Masterthesis\results\baseline_cot\arc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508EED0D-AC83-4951-A11B-3DB699FF0DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEC48CB-66C6-40FC-AB76-C949FF1C767E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="6" xr2:uid="{0EC1F964-009C-44AA-8331-5AE0B72718BA}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{0EC1F964-009C-44AA-8331-5AE0B72718BA}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="76">
   <si>
     <t>task_name</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>b1948b0a.json</t>
+  </si>
+  <si>
+    <t>test_description_correct_and_complete</t>
   </si>
 </sst>
 </file>
@@ -927,9 +930,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C160EF6F-0555-4875-ACB1-014D97C824DF}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +994,7 @@
         <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>31</v>
@@ -1606,9 +1609,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1645F0D-2C42-4FDA-9EAC-EE98B635BBCE}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,7 +1673,7 @@
         <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>31</v>
@@ -2319,9 +2322,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687D7031-258F-4DE2-A9D8-7479C0C678CF}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S8" sqref="S8"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,7 +2386,7 @@
         <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>31</v>
@@ -2597,11 +2600,11 @@
         <v>1</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" ref="D3:D11" si="0">IF(C5=TRUE,"None","")</f>
+        <f t="shared" ref="D5" si="0">IF(C5=TRUE,"None","")</f>
         <v>None</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" ref="E3:E11" si="1">IF(C5=TRUE,"None","")</f>
+        <f t="shared" ref="E5" si="1">IF(C5=TRUE,"None","")</f>
         <v>None</v>
       </c>
       <c r="F5" t="b">
@@ -3005,9 +3008,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E115DF2E-9FD7-45D2-9A69-FF89490FCD4C}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD21"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3069,7 +3072,7 @@
         <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>31</v>
@@ -3167,11 +3170,11 @@
         <v>1</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D21" si="0">IF(C3=TRUE,"None","")</f>
+        <f t="shared" ref="D3" si="0">IF(C3=TRUE,"None","")</f>
         <v>None</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E21" si="1">IF(C3=TRUE,"None","")</f>
+        <f t="shared" ref="E3" si="1">IF(C3=TRUE,"None","")</f>
         <v>None</v>
       </c>
       <c r="F3" t="b">
@@ -3187,7 +3190,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J21" si="2">IF(I3=TRUE,"None","")</f>
+        <f t="shared" ref="J3" si="2">IF(I3=TRUE,"None","")</f>
         <v>None</v>
       </c>
       <c r="K3" t="b">
@@ -3209,7 +3212,7 @@
         <v>1</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q21" si="3">IF(P3=TRUE,"None","")</f>
+        <f t="shared" ref="Q3" si="3">IF(P3=TRUE,"None","")</f>
         <v>None</v>
       </c>
       <c r="R3" t="b">
@@ -3226,9 +3229,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A598A86-A726-4035-A5D8-7FB05BCB0D54}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3290,7 +3293,7 @@
         <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>31</v>
@@ -3608,11 +3611,11 @@
         <v>1</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" ref="D3:D11" si="0">IF(C7=TRUE,"None","")</f>
+        <f t="shared" ref="D7" si="0">IF(C7=TRUE,"None","")</f>
         <v>None</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" ref="E3:E11" si="1">IF(C7=TRUE,"None","")</f>
+        <f t="shared" ref="E7" si="1">IF(C7=TRUE,"None","")</f>
         <v>None</v>
       </c>
       <c r="F7" t="b">
@@ -3892,9 +3895,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE99220F-96BB-4653-9C1B-82FB7B184800}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3956,7 +3959,7 @@
         <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>31</v>
@@ -4090,7 +4093,7 @@
         <v>1</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q21" si="0">IF(P3=TRUE,"None","")</f>
+        <f t="shared" ref="Q3:Q5" si="0">IF(P3=TRUE,"None","")</f>
         <v>None</v>
       </c>
       <c r="R3" t="b">

</xml_diff>